<commit_message>
added scada tag conversion
</commit_message>
<xml_diff>
--- a/Tag_Builder/Input/SCADA_TAGS.xlsx
+++ b/Tag_Builder/Input/SCADA_TAGS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F185846B-A3E6-D848-8467-16EC26008D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E3C358-5023-D644-92E8-C28F196EE652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="500" windowWidth="17080" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51400" yWindow="500" windowWidth="24360" windowHeight="19820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDH" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21723" uniqueCount="2210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21726" uniqueCount="2211">
   <si>
     <t>[BLOCK TYPE</t>
   </si>
@@ -6632,9 +6632,6 @@
     <t>IR111</t>
   </si>
   <si>
-    <t>DM411</t>
-  </si>
-  <si>
     <t>IR112</t>
   </si>
   <si>
@@ -6648,6 +6645,12 @@
   </si>
   <si>
     <t>DM510</t>
+  </si>
+  <si>
+    <t>New_Address</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -6701,7 +6704,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="20">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -6772,35 +6781,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3247C6DC-223E-A348-97FD-D1CDBB6A2B97}" name="Table1" displayName="Table1" ref="A1:G297" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:G297" xr:uid="{3247C6DC-223E-A348-97FD-D1CDBB6A2B97}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{37113169-19DD-AA4B-808E-1AA6B2C48B10}" name="Type" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{B6EBA282-F8B0-6746-8952-B2216910D340}" name="TAG" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{3CF6B033-FF0B-664B-A4CD-4FCB70CF89CC}" name="NEXT BLK" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{0B4E7010-94B7-E544-8073-C942C9FEBD3D}" name="DESCRIPTION" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{98852D7F-957C-5C4E-96B8-BA0418CA0B40}" name="Full Address" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{7662D4FD-AA70-C64E-AEED-F5F23763383D}" name="Clean_Address_BCD" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{D28F73D7-5A82-FC43-AB09-FCF76AD9E53D}" name="Clean_Address" dataDxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3247C6DC-223E-A348-97FD-D1CDBB6A2B97}" name="Table1" displayName="Table1" ref="A1:H297" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:H297" xr:uid="{3247C6DC-223E-A348-97FD-D1CDBB6A2B97}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{37113169-19DD-AA4B-808E-1AA6B2C48B10}" name="Type" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{B6EBA282-F8B0-6746-8952-B2216910D340}" name="TAG" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{3CF6B033-FF0B-664B-A4CD-4FCB70CF89CC}" name="NEXT BLK" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{0B4E7010-94B7-E544-8073-C942C9FEBD3D}" name="DESCRIPTION" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{98852D7F-957C-5C4E-96B8-BA0418CA0B40}" name="Full Address" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{7662D4FD-AA70-C64E-AEED-F5F23763383D}" name="Clean_Address_BCD" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{D28F73D7-5A82-FC43-AB09-FCF76AD9E53D}" name="Clean_Address" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{58AD2E1C-79BD-B346-BE3E-51AEDB046035}" name="New_Address" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8998A05B-2A2C-624A-BA23-A1CAF529A8D5}" name="Table2" displayName="Table2" ref="A1:G211" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G211" xr:uid="{8998A05B-2A2C-624A-BA23-A1CAF529A8D5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8998A05B-2A2C-624A-BA23-A1CAF529A8D5}" name="Table2" displayName="Table2" ref="A1:H211" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:H211" xr:uid="{8998A05B-2A2C-624A-BA23-A1CAF529A8D5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G211">
     <sortCondition ref="G1:G211"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1ED72638-1FC7-4C44-AB38-58B91840E8A0}" name="Type" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{337EB105-1426-C645-BB0A-E4753BBE7682}" name="TAG" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{4E9D2C31-EDDD-C64C-BFB5-1D5F13955863}" name="NEXT BLK" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{B0D0C8B0-957A-E34C-9299-EC78C12A8D74}" name="DESCRIPTION" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{0080EC75-5246-EF41-AD71-EB65AEC8D029}" name="Full Address" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{25C233D7-6627-AB41-A589-26253C52FB0B}" name="Clean_Address_BCD" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{148B53D2-FF41-4849-9857-8C0EB9091A8D}" name="Clean_Address" dataDxfId="0"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{1ED72638-1FC7-4C44-AB38-58B91840E8A0}" name="Type" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{337EB105-1426-C645-BB0A-E4753BBE7682}" name="TAG" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{4E9D2C31-EDDD-C64C-BFB5-1D5F13955863}" name="NEXT BLK" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{B0D0C8B0-957A-E34C-9299-EC78C12A8D74}" name="DESCRIPTION" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{0080EC75-5246-EF41-AD71-EB65AEC8D029}" name="Full Address" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{25C233D7-6627-AB41-A589-26253C52FB0B}" name="Clean_Address_BCD" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{148B53D2-FF41-4849-9857-8C0EB9091A8D}" name="Clean_Address" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{C34F215C-8E3B-6D47-897B-AB6CD6C9CBA9}" name="New_Address" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -53798,8 +53809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB84D61-5F99-9F49-A52E-1F5039ED1CBF}">
   <dimension ref="A1:DB297"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187"/>
+    <sheetView topLeftCell="C1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53927,6 +53938,9 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>1810</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2209</v>
       </c>
     </row>
     <row r="2" spans="1:68" x14ac:dyDescent="0.2">
@@ -92864,8 +92878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D156082-C62D-FA48-B103-C7B6A124D982}">
   <dimension ref="A1:DF211"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E173" sqref="E173"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -93000,6 +93014,9 @@
       <c r="G1" s="1" t="s">
         <v>1810</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>2209</v>
+      </c>
     </row>
     <row r="2" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -93018,7 +93035,10 @@
         <v>2035</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>2204</v>
+        <v>1885</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2210</v>
       </c>
       <c r="M2" s="2"/>
       <c r="AY2" s="2"/>
@@ -93099,7 +93119,7 @@
         <v>2165</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="M5" s="2"/>
       <c r="AY5" s="2"/>
@@ -93125,7 +93145,7 @@
         <v>2162</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
       <c r="M6" s="2"/>
       <c r="T6" s="2"/>
@@ -93153,7 +93173,7 @@
         <v>2167</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2"/>
@@ -93177,7 +93197,7 @@
         <v>2167</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="M8" s="2"/>
       <c r="T8" s="2"/>
@@ -93300,7 +93320,7 @@
         <v>2168</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
       <c r="M13" s="3"/>
       <c r="T13" s="3"/>
@@ -94024,7 +94044,7 @@
         <v>2159</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="AS43" s="2"/>
       <c r="AT43" s="2"/>

</xml_diff>